<commit_message>
-- Pandas -- Updated the dummy class data files. Removed dummy_class and replaced it with two files with the data split.
</commit_message>
<xml_diff>
--- a/pandas-data/dummy-class-2-of-2.xlsx
+++ b/pandas-data/dummy-class-2-of-2.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
-  <si>
-    <t xml:space="preserve">This is a dummy set of data created to show how to work with dataframes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Student No</t>
   </si>
@@ -82,9 +79,6 @@
     <t xml:space="preserve">A1218599T</t>
   </si>
   <si>
-    <t xml:space="preserve">A7210476B</t>
-  </si>
-  <si>
     <t xml:space="preserve">A1512479K</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t xml:space="preserve">A5975988J</t>
   </si>
   <si>
-    <t xml:space="preserve">A3699958T</t>
-  </si>
-  <si>
     <t xml:space="preserve">A1956366U</t>
   </si>
   <si>
@@ -127,13 +118,7 @@
     <t xml:space="preserve">A3217320C</t>
   </si>
   <si>
-    <t xml:space="preserve">A6867791C</t>
-  </si>
-  <si>
     <t xml:space="preserve">A4080490P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A7667457P</t>
   </si>
 </sst>
 </file>
@@ -263,10 +248,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="U18" activeCellId="0" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -277,17 +262,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>21.25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,7 +282,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>21.25</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,7 +290,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>18.75</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,7 +298,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43.75</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,7 +306,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>18.75</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,7 +314,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>17.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,7 +322,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>32.5</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,7 +330,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>31.25</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,7 +338,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>43.75</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,7 +346,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>47.5</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +354,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>41.25</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,7 +362,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>32.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,7 +370,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>50</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,7 +378,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>41.25</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,7 +386,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,7 +394,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,7 +402,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,20 +410,23 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>50</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B20" s="1" t="n">
+        <v>43.75</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>33.75</v>
+        <v>46.25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +434,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>43.75</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,7 +442,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>46.25</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +450,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>32.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,7 +458,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>41.25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,7 +466,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>22.5</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,7 +474,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>30</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,7 +482,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>47.5</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,7 +490,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>31.25</v>
+        <v>28.75</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,56 +498,30 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>16.25</v>
+        <v>36.25</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B31" s="1" t="n">
+        <v>16.25</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>28.75</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>36.25</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="1" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>